<commit_message>
add thd 256, 512 to AWS charts
</commit_message>
<xml_diff>
--- a/AWS/Sysbench_AWS_PG15_8C32G.xlsx
+++ b/AWS/Sysbench_AWS_PG15_8C32G.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demai/work/sysbenchCloudDB/AWS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0695B3E1-938D-B448-819C-4F8EA9BA57FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E1C5CB-E24F-784D-9F79-07FE0AFD8D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12640" yWindow="1080" windowWidth="23140" windowHeight="19400" xr2:uid="{1C006222-4FFB-AD41-A2F8-DEE8063218B2}"/>
+    <workbookView xWindow="25100" yWindow="500" windowWidth="23140" windowHeight="19400" xr2:uid="{1C006222-4FFB-AD41-A2F8-DEE8063218B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -271,10 +271,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$8</c:f>
+              <c:f>Sheet1!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.32616742786381003</c:v>
                 </c:pt>
@@ -295,6 +295,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.8591763092368943</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0551257639711857</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7646502709684291</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -348,10 +354,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -372,16 +378,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>244.95499999999998</c:v>
                 </c:pt>
@@ -402,6 +414,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1396.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1543.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1325.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -841,9 +859,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>p95 (ms)</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>
@@ -856,10 +871,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -880,16 +895,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>11.96</c:v>
                 </c:pt>
@@ -910,6 +931,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>136.17000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>248.83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>746.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -964,10 +991,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -988,16 +1015,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:f>Sheet1!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.1</c:v>
                 </c:pt>
@@ -1018,6 +1051,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2939,7 +2978,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
revisit AWS by increasing IOPS from 2K to 4K
</commit_message>
<xml_diff>
--- a/AWS/Sysbench_AWS_PG15_8C32G.xlsx
+++ b/AWS/Sysbench_AWS_PG15_8C32G.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demai/work/sysbenchCloudDB/AWS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E1C5CB-E24F-784D-9F79-07FE0AFD8D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DAAFA1-3273-2D4E-8692-37427583008B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25100" yWindow="500" windowWidth="23140" windowHeight="19400" xr2:uid="{1C006222-4FFB-AD41-A2F8-DEE8063218B2}"/>
+    <workbookView xWindow="22600" yWindow="500" windowWidth="23140" windowHeight="19400" xr2:uid="{1C006222-4FFB-AD41-A2F8-DEE8063218B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -859,6 +859,17 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P95 latency (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>

</xml_diff>